<commit_message>
Kontakt bearbeiten und hinzufügen
</commit_message>
<xml_diff>
--- a/Franz_Zeitaufwand.xlsx
+++ b/Franz_Zeitaufwand.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franz Kautz\Documents\GitHub\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franz Kautz\Documents\GitHub\NEU-VHS_Anwendungsprogramm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A28F65-E95F-4C4F-BF72-611C5AF494EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A505DBC9-609F-4388-8C99-973525387D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6E9365D-C463-4060-9B1C-52DA4287FA0A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Zeitliste Maturaprojekt</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Problembehandlung (GitHub), Organisatorisches</t>
+  </si>
+  <si>
+    <t>Kontakt hinzufügen, bearbeiten</t>
+  </si>
+  <si>
+    <t>Organisatorisches; Kontakt hinzufügen, bearbeiten</t>
   </si>
 </sst>
 </file>
@@ -596,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FFF525-C120-47EA-85C2-D95098222D0B}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,7 +638,7 @@
       </c>
       <c r="F3">
         <f>SUM(C4:C100)</f>
-        <v>127</v>
+        <v>131.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -650,7 +656,7 @@
       </c>
       <c r="F4">
         <f>180-F3</f>
-        <v>53</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1003,6 +1009,28 @@
       </c>
       <c r="C36">
         <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>43845</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>43846</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kurs anlegen; Kontakt anlegen
</commit_message>
<xml_diff>
--- a/Franz_Zeitaufwand.xlsx
+++ b/Franz_Zeitaufwand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franz Kautz\Documents\GitHub\NEU-VHS_Anwendungsprogramm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A505DBC9-609F-4388-8C99-973525387D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DA614E-C4C4-498D-9E75-45169E60A12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6E9365D-C463-4060-9B1C-52DA4287FA0A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Zeitliste Maturaprojekt</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Organisatorisches; Kontakt hinzufügen, bearbeiten</t>
+  </si>
+  <si>
+    <t>Fehlersuche; überlegen über was ich alles schreiben kann</t>
   </si>
 </sst>
 </file>
@@ -602,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FFF525-C120-47EA-85C2-D95098222D0B}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,7 +641,7 @@
       </c>
       <c r="F3">
         <f>SUM(C4:C100)</f>
-        <v>131.5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -656,7 +659,7 @@
       </c>
       <c r="F4">
         <f>180-F3</f>
-        <v>48.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,6 +1033,17 @@
         <v>37</v>
       </c>
       <c r="C38">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>43847</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kontakt bearbeiten; Kursort anzeigen, bearbeiten, anlegen; Teilnehmer anzeigen; offene Posten anzeigen
</commit_message>
<xml_diff>
--- a/Franz_Zeitaufwand.xlsx
+++ b/Franz_Zeitaufwand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franz Kautz\Documents\GitHub\NEU-VHS_Anwendungsprogramm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DA614E-C4C4-498D-9E75-45169E60A12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF75BC06-1632-4876-A874-28B8F07D2671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6E9365D-C463-4060-9B1C-52DA4287FA0A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Zeitliste Maturaprojekt</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Fehlersuche; überlegen über was ich alles schreiben kann</t>
+  </si>
+  <si>
+    <t>Kursleiter anzeigen; Kursort anzeigen, bearbeiten, anlegen; Teilnehmer anzeigen; offene Posten anzeigen</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FFF525-C120-47EA-85C2-D95098222D0B}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +644,7 @@
       </c>
       <c r="F3">
         <f>SUM(C4:C100)</f>
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -659,7 +662,7 @@
       </c>
       <c r="F4">
         <f>180-F3</f>
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1045,6 +1048,17 @@
       </c>
       <c r="C39">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>43848</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KursleiterKurs und KontaktKurs angefangen
</commit_message>
<xml_diff>
--- a/Franz_Zeitaufwand.xlsx
+++ b/Franz_Zeitaufwand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franz Kautz\Documents\GitHub\NEU-VHS_Anwendungsprogramm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956BF719-85D5-4033-A225-EA07DF9CC8C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58A1C76-0069-45A9-B8F1-3617363B2FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{C6E9365D-C463-4060-9B1C-52DA4287FA0A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6E9365D-C463-4060-9B1C-52DA4287FA0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Zeitliste Maturaprojekt</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Kursleiter bearbeiten</t>
+  </si>
+  <si>
+    <t>Kursbuchung überlegen wie ich das mach, design in visual studio</t>
   </si>
 </sst>
 </file>
@@ -622,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FFF525-C120-47EA-85C2-D95098222D0B}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +659,7 @@
       </c>
       <c r="F3">
         <f>SUM(C4:C100)</f>
-        <v>148.5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -674,7 +677,7 @@
       </c>
       <c r="F4">
         <f>180-F3</f>
-        <v>31.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1114,12 +1117,18 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>43862</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
       <c r="C45">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>